<commit_message>
Added final copy of correction grid.
</commit_message>
<xml_diff>
--- a/documentation/correctiongrid-FINAL-VERSION.xlsx
+++ b/documentation/correctiongrid-FINAL-VERSION.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="233">
   <si>
     <t>Iteration 2 Tentative final correction grid for Iteration 2</t>
   </si>
@@ -702,6 +702,10 @@
     <t>quality of unbound UCMs</t>
   </si>
   <si>
+    <t>This isn't a yes or no question
+</t>
+  </si>
+  <si>
     <t>traceability of unbound UCMs to Ucs</t>
   </si>
   <si>
@@ -712,6 +716,9 @@
   </si>
   <si>
     <t>PLEASE list any other extra features below, each with a short description</t>
+  </si>
+  <si>
+    <t>More thatn minimum giant monster, multi combat,  limited players playing simultaneously (birdsong), more than requried treasures/group characters.</t>
   </si>
 </sst>
 </file>
@@ -2177,19 +2184,25 @@
       <c r="A147" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="B147" s="2"/>
+      <c r="B147" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="148" ht="15.75" customHeight="1">
       <c r="A148" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="B148" s="2"/>
+      <c r="B148" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="149" ht="15.75" customHeight="1">
       <c r="A149" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="B149" s="2"/>
+      <c r="B149" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="150" ht="15.75" customHeight="1">
       <c r="A150" s="2" t="s">
@@ -2201,85 +2214,113 @@
       <c r="A151" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="B151" s="2"/>
+      <c r="B151" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="152" ht="15.75" customHeight="1">
       <c r="A152" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="B152" s="2"/>
+      <c r="B152" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="153" ht="15.75" customHeight="1">
       <c r="A153" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="B153" s="2"/>
+      <c r="B153" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="154" ht="15.75" customHeight="1">
       <c r="A154" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="B154" s="2"/>
+      <c r="B154" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="155" ht="15.75" customHeight="1">
       <c r="A155" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="B155" s="2"/>
+      <c r="B155" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="156" ht="15.75" customHeight="1">
       <c r="A156" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="B156" s="2"/>
+      <c r="B156" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="157" ht="15.75" customHeight="1">
       <c r="A157" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="B157" s="2"/>
+      <c r="B157" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="158" ht="15.75" customHeight="1">
       <c r="A158" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="B158" s="2"/>
+      <c r="B158" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="159" ht="15.75" customHeight="1">
       <c r="A159" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="B159" s="2"/>
+      <c r="B159" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="160" ht="15.75" customHeight="1">
       <c r="A160" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="B160" s="2"/>
+      <c r="B160" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="161" ht="15.75" customHeight="1">
       <c r="A161" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="B161" s="2"/>
+      <c r="B161" s="3" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="162" ht="15.75" customHeight="1">
       <c r="A162" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="B162" s="2"/>
+        <v>228</v>
+      </c>
+      <c r="B162" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="163" ht="15.75" customHeight="1">
       <c r="A163" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="B163" s="2"/>
+        <v>229</v>
+      </c>
+      <c r="B163" s="3" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="164" ht="15.75" customHeight="1">
       <c r="A164" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="B164" s="2"/>
+        <v>230</v>
+      </c>
+      <c r="B164" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="165" ht="15.75" customHeight="1">
       <c r="A165" s="2"/>
@@ -2287,9 +2328,11 @@
     </row>
     <row r="166" ht="15.75" customHeight="1">
       <c r="A166" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="B166" s="2"/>
+        <v>231</v>
+      </c>
+      <c r="B166" s="3" t="s">
+        <v>232</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>